<commit_message>
added tertile thresholding comparison for 09
</commit_message>
<xml_diff>
--- a/Publication/Outputs/Tables/ST4.xlsx
+++ b/Publication/Outputs/Tables/ST4.xlsx
@@ -1,125 +1,100 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10216"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JoshsMacbook2015/Desktop/grady-bcvi-calculator/Publication/Outputs/Tables/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B405E8A-49D0-624D-88DC-39133F63D020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="42280" yWindow="-3080" windowWidth="17540" windowHeight="12140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
-  <si>
-    <t>Risk Stratum</t>
-  </si>
-  <si>
-    <t>N Patients (%)</t>
-  </si>
-  <si>
-    <t>Observed Strokes</t>
-  </si>
-  <si>
-    <t>Sensitivity</t>
-  </si>
-  <si>
-    <t>Specificity</t>
-  </si>
-  <si>
-    <t>PPV</t>
-  </si>
-  <si>
-    <t>NPV</t>
-  </si>
-  <si>
-    <t>Low (&lt;10%)</t>
-  </si>
-  <si>
-    <t>512 (43%)</t>
-  </si>
-  <si>
-    <t>6 (1%)</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Moderate (10-30%)</t>
-  </si>
-  <si>
-    <t>550 (46%)</t>
-  </si>
-  <si>
-    <t>19 (3%)</t>
-  </si>
-  <si>
-    <t>88%</t>
-  </si>
-  <si>
-    <t>44%</t>
-  </si>
-  <si>
-    <t>7%</t>
-  </si>
-  <si>
-    <t>99%</t>
-  </si>
-  <si>
-    <t>High (≥30%)</t>
-  </si>
-  <si>
-    <t>135 (11%)</t>
-  </si>
-  <si>
-    <t>27 (20%)</t>
-  </si>
-  <si>
-    <t>52%</t>
-  </si>
-  <si>
-    <t>91%</t>
-  </si>
-  <si>
-    <t>20%</t>
-  </si>
-  <si>
-    <t>98%</t>
-  </si>
-  <si>
-    <t>Overall Population</t>
-  </si>
-  <si>
-    <t>1197</t>
-  </si>
-  <si>
-    <t>52 (4%)</t>
-  </si>
-  <si>
-    <t>69%</t>
-  </si>
-  <si>
-    <t>75%</t>
-  </si>
-  <si>
-    <t>11%</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+  <si>
+    <t xml:space="preserve">Risk Stratum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N Patients (%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Observed Strokes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sensitivity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specificity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PPV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NPV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Low (&lt;10%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">512 (43%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 (1%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moderate (10-30%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">550 (46%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19 (3%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">44%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High (≥30%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">135 (11%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27 (20%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">52%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">91%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">98%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -155,15 +130,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -445,23 +411,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <selection activeCell="G5" sqref="B2:G5"/>
-    </sheetView>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="4.5" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -484,7 +441,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -507,7 +464,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -530,7 +487,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -550,34 +507,11 @@
         <v>23</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>